<commit_message>
corrections + jeu symétrique face à la banque
</commit_message>
<xml_diff>
--- a/policy_vsIA.xlsx
+++ b/policy_vsIA.xlsx
@@ -555,8 +555,8 @@
       <c r="D4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="n">
-        <v>2</v>
+      <c r="E4" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>1</v>
@@ -564,8 +564,8 @@
       <c r="G4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>1</v>
+      <c r="H4" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="I4" s="4" t="n">
         <v>0</v>
@@ -588,8 +588,8 @@
       <c r="O4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P4" s="4" t="n">
-        <v>0</v>
+      <c r="P4" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -599,26 +599,26 @@
       <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>2</v>
+      <c r="C5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>0</v>
+      <c r="H5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J5" s="4" t="n">
         <v>0</v>
@@ -629,8 +629,8 @@
       <c r="L5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="4" t="n">
-        <v>0</v>
+      <c r="M5" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="N5" s="4" t="n">
         <v>0</v>
@@ -638,8 +638,8 @@
       <c r="O5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P5" s="3" t="n">
-        <v>2</v>
+      <c r="P5" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -649,29 +649,29 @@
       <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>1</v>
+      <c r="C6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4" t="n">
-        <v>0</v>
+      <c r="F6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="I6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="3" t="n">
-        <v>2</v>
+      <c r="J6" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="K6" s="4" t="n">
         <v>0</v>
@@ -696,32 +696,32 @@
       <c r="A7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>1</v>
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <v>0</v>
+      <c r="E7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="G7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4" t="n">
-        <v>0</v>
+      <c r="H7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="K7" s="4" t="n">
         <v>0</v>
@@ -761,23 +761,23 @@
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>1</v>
+      <c r="G8" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="K8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="L8" s="4" t="n">
-        <v>0</v>
+      <c r="L8" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="M8" s="4" t="n">
         <v>0</v>
@@ -788,40 +788,40 @@
       <c r="O8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P8" s="4" t="n">
-        <v>0</v>
+      <c r="P8" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>2</v>
+      <c r="B9" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>0</v>
+      <c r="E9" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H9" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4" t="n">
-        <v>0</v>
+      <c r="H9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="K9" s="4" t="n">
         <v>0</v>
@@ -838,8 +838,8 @@
       <c r="O9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="3" t="n">
-        <v>2</v>
+      <c r="P9" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -861,20 +861,20 @@
       <c r="F10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="4" t="n">
-        <v>0</v>
+      <c r="G10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H10" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="4" t="n">
-        <v>0</v>
+      <c r="I10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="L10" s="4" t="n">
         <v>0</v>
@@ -896,11 +896,11 @@
       <c r="A11" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>1</v>
+      <c r="B11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>1</v>
@@ -914,17 +914,17 @@
       <c r="G11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="4" t="n">
-        <v>0</v>
+      <c r="H11" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>1</v>
+      <c r="J11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="L11" s="4" t="n">
         <v>0</v>
@@ -938,8 +938,8 @@
       <c r="O11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P11" s="3" t="n">
-        <v>2</v>
+      <c r="P11" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -958,8 +958,8 @@
       <c r="E12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="3" t="n">
-        <v>2</v>
+      <c r="F12" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>1</v>
@@ -967,11 +967,11 @@
       <c r="H12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4" t="n">
-        <v>0</v>
+      <c r="I12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="K12" s="4" t="n">
         <v>0</v>
@@ -988,8 +988,8 @@
       <c r="O12" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P12" s="4" t="n">
-        <v>0</v>
+      <c r="P12" s="2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1011,14 +1011,14 @@
       <c r="F13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="4" t="n">
-        <v>0</v>
+      <c r="G13" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <v>1</v>
+      <c r="I13" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="J13" s="2" t="n">
         <v>1</v>
@@ -1038,8 +1038,8 @@
       <c r="O13" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="P13" s="2" t="n">
-        <v>1</v>
+      <c r="P13" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1090,17 +1090,17 @@
       <c r="B18" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>1</v>
+      <c r="C18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="3" t="n">
-        <v>2</v>
+      <c r="F18" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="G18" s="4" t="n">
         <v>0</v>
@@ -1108,8 +1108,8 @@
       <c r="H18" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="2" t="n">
-        <v>1</v>
+      <c r="I18" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="J18" s="4" t="n">
         <v>0</v>
@@ -1119,14 +1119,14 @@
       <c r="A19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B19" s="3" t="n">
-        <v>2</v>
+      <c r="B19" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D19" s="4" t="n">
-        <v>0</v>
+      <c r="D19" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>0</v>
@@ -1134,8 +1134,8 @@
       <c r="F19" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="4" t="n">
-        <v>0</v>
+      <c r="G19" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="H19" s="4" t="n">
         <v>0</v>
@@ -1151,29 +1151,29 @@
       <c r="A20" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B20" s="2" t="n">
-        <v>1</v>
+      <c r="B20" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="4" t="n">
-        <v>0</v>
+      <c r="D20" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="F20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3" t="n">
-        <v>2</v>
+      <c r="F20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H20" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="3" t="n">
-        <v>2</v>
+      <c r="I20" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="J20" s="4" t="n">
         <v>0</v>
@@ -1183,23 +1183,23 @@
       <c r="A21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4" t="n">
-        <v>0</v>
+      <c r="B21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="3" t="n">
-        <v>2</v>
+      <c r="G21" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="H21" s="4" t="n">
         <v>0</v>
@@ -1215,29 +1215,29 @@
       <c r="A22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B22" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>2</v>
+      <c r="B22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F22" s="2" t="n">
-        <v>1</v>
+      <c r="F22" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="G22" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="H22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>1</v>
+      <c r="H22" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="J22" s="4" t="n">
         <v>0</v>
@@ -1247,11 +1247,11 @@
       <c r="A23" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>1</v>
+      <c r="B23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>1</v>
@@ -1259,8 +1259,8 @@
       <c r="E23" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="3" t="n">
-        <v>2</v>
+      <c r="F23" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="G23" s="3" t="n">
         <v>2</v>
@@ -1268,8 +1268,8 @@
       <c r="H23" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I23" s="3" t="n">
-        <v>2</v>
+      <c r="I23" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="J23" s="4" t="n">
         <v>0</v>
@@ -1282,23 +1282,23 @@
       <c r="B24" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3" t="n">
-        <v>2</v>
+      <c r="C24" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="G24" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="H24" s="4" t="n">
-        <v>0</v>
+      <c r="H24" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>0</v>
@@ -1314,8 +1314,8 @@
       <c r="B25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="4" t="n">
-        <v>0</v>
+      <c r="C25" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>1</v>
@@ -1343,8 +1343,8 @@
       <c r="A26" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B26" s="2" t="n">
-        <v>1</v>
+      <c r="B26" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
@@ -1358,8 +1358,8 @@
       <c r="F26" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G26" s="3" t="n">
-        <v>2</v>
+      <c r="G26" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="H26" s="4" t="n">
         <v>0</v>
@@ -1390,8 +1390,8 @@
       <c r="F27" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>1</v>
+      <c r="G27" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="H27" s="4" t="n">
         <v>0</v>
@@ -1457,17 +1457,17 @@
       <c r="C32" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D32" s="2" t="n">
-        <v>1</v>
+      <c r="D32" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F32" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="4" t="n">
-        <v>0</v>
+      <c r="F32" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="H32" s="2" t="n">
         <v>1</v>
@@ -1486,14 +1486,14 @@
       <c r="A33" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B33" s="3" t="n">
-        <v>2</v>
+      <c r="B33" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D33" s="2" t="n">
-        <v>1</v>
+      <c r="D33" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>1</v>
@@ -1510,8 +1510,8 @@
       <c r="I33" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="J33" s="5" t="n">
-        <v>3</v>
+      <c r="J33" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="K33" s="5" t="n">
         <v>3</v>
@@ -1527,8 +1527,8 @@
       <c r="C34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D34" s="3" t="n">
-        <v>2</v>
+      <c r="D34" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>1</v>
@@ -1559,23 +1559,23 @@
       <c r="B35" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C35" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>1</v>
+      <c r="C35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G35" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="5" t="n">
-        <v>3</v>
+      <c r="G35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="I35" s="4" t="n">
         <v>0</v>
@@ -1591,26 +1591,26 @@
       <c r="A36" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B36" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="3" t="n">
-        <v>2</v>
+      <c r="B36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="F36" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H36" s="4" t="n">
-        <v>0</v>
+      <c r="G36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="I36" s="5" t="n">
         <v>3</v>
@@ -1629,11 +1629,11 @@
       <c r="B37" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C37" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3" t="n">
-        <v>2</v>
+      <c r="C37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>1</v>
@@ -1641,8 +1641,8 @@
       <c r="F37" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G37" s="3" t="n">
-        <v>2</v>
+      <c r="G37" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="H37" s="4" t="n">
         <v>0</v>
@@ -1664,8 +1664,8 @@
       <c r="B38" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C38" s="3" t="n">
-        <v>2</v>
+      <c r="C38" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D38" s="2" t="n">
         <v>1</v>
@@ -1673,20 +1673,20 @@
       <c r="E38" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F38" s="3" t="n">
-        <v>2</v>
+      <c r="F38" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H38" s="3" t="n">
-        <v>2</v>
+      <c r="H38" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="I38" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="J38" s="4" t="n">
-        <v>0</v>
+      <c r="J38" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="K38" s="5" t="n">
         <v>3</v>
@@ -1696,11 +1696,11 @@
       <c r="A39" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B39" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="2" t="n">
-        <v>1</v>
+      <c r="B39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>1</v>
@@ -1708,14 +1708,14 @@
       <c r="E39" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F39" s="2" t="n">
-        <v>1</v>
+      <c r="F39" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H39" s="4" t="n">
-        <v>0</v>
+      <c r="H39" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="I39" s="2" t="n">
         <v>1</v>
@@ -1731,8 +1731,8 @@
       <c r="A40" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B40" s="4" t="n">
-        <v>0</v>
+      <c r="B40" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>1</v>
@@ -1749,11 +1749,11 @@
       <c r="G40" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H40" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="4" t="n">
-        <v>0</v>
+      <c r="H40" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J40" s="4" t="n">
         <v>0</v>
@@ -1766,8 +1766,8 @@
       <c r="A41" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B41" s="2" t="n">
-        <v>1</v>
+      <c r="B41" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>1</v>
@@ -1784,11 +1784,11 @@
       <c r="G41" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H41" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="4" t="n">
-        <v>0</v>
+      <c r="H41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J41" s="4" t="n">
         <v>0</v>

</xml_diff>